<commit_message>
Commit preventivo por que quitare el forloop de la Nentrada y Nsalida
</commit_message>
<xml_diff>
--- a/polls/static/polls/Datos/Inventario.xlsx
+++ b/polls/static/polls/Datos/Inventario.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>CLASIF.EQUIP(ID)</t>
   </si>
@@ -47,6 +47,15 @@
     <t>hola crayola</t>
   </si>
   <si>
+    <t>power300</t>
+  </si>
+  <si>
+    <t>antena</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
     <t>Num de Factura</t>
   </si>
   <si>
@@ -120,6 +129,75 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>2018-11-09</t>
+  </si>
+  <si>
+    <t>sadas</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>2018-11-17</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>haber haber</t>
+  </si>
+  <si>
+    <t>2018-11-10</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2018-11-03</t>
+  </si>
+  <si>
+    <t>Esta bien bonito</t>
+  </si>
+  <si>
+    <t>2018-11-16</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0123</t>
+  </si>
+  <si>
+    <t>2018-11-02</t>
+  </si>
+  <si>
+    <t>instaLACION</t>
+  </si>
+  <si>
+    <t>5253</t>
+  </si>
+  <si>
+    <t>OSCAR</t>
+  </si>
+  <si>
+    <t>01486513847</t>
+  </si>
+  <si>
+    <t>ewg</t>
+  </si>
+  <si>
+    <t>23131614510230</t>
   </si>
 </sst>
 </file>
@@ -600,7 +678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -653,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F2" s="7" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -677,6 +755,46 @@
       </c>
       <c r="F3" s="7" t="n">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -712,33 +830,33 @@
   <sheetData>
     <row customFormat="1" customHeight="1" ht="33.75" r="1" s="3" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -750,10 +868,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -785,7 +903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -805,39 +923,39 @@
   <sheetData>
     <row customFormat="1" customHeight="1" ht="33" r="1" s="3" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -849,24 +967,24 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -878,16 +996,219 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
         <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Todo el modulo de entrada por lotes casi listo solo faltaria el post que agregaria los datos
</commit_message>
<xml_diff>
--- a/polls/static/polls/Datos/Inventario.xlsx
+++ b/polls/static/polls/Datos/Inventario.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Israel\Desktop\tutorial\mysite\polls\static\polls\Datos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="7680"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7680" windowWidth="10170" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="inventario" sheetId="1" r:id="rId1"/>
-    <sheet name="Entradas" sheetId="2" r:id="rId2"/>
-    <sheet name="Salidas" sheetId="3" r:id="rId3"/>
+    <sheet name="inventario" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Entradas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Salidas" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Inventario">Tabla31[]</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>CLASIF.EQUIP(ID)</t>
   </si>
@@ -42,6 +36,24 @@
   </si>
   <si>
     <t>Stock</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Carro</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Trailer</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Ford Focus</t>
   </si>
   <si>
     <t>Num de Factura</t>
@@ -80,19 +92,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,39 +121,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
@@ -174,7 +187,7 @@
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
+      <numFmt formatCode=";;;" numFmtId="164"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
@@ -231,67 +244,59 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla31" displayName="Tabla31" ref="A1:F3" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="27" displayName="Tabla31" headerRowCount="1" headerRowDxfId="28" id="1" name="Tabla31" ref="A1:F3" totalsRowDxfId="26">
   <autoFilter ref="A1:F3"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="CLASIF.EQUIP(ID)" totalsRowLabel="Total" dataDxfId="25"/>
-    <tableColumn id="2" name="Descripcion" dataDxfId="24"/>
-    <tableColumn id="3" name="Existencias Iniciales" dataDxfId="23"/>
-    <tableColumn id="4" name="Entradas" dataDxfId="22"/>
-    <tableColumn id="5" name="Salidas" dataDxfId="21"/>
-    <tableColumn id="6" name="Stock" totalsRowFunction="sum" dataDxfId="20"/>
+    <tableColumn dataDxfId="25" id="1" name="CLASIF.EQUIP(ID)" totalsRowLabel="Total"/>
+    <tableColumn dataDxfId="24" id="2" name="Descripcion"/>
+    <tableColumn dataDxfId="23" id="3" name="Existencias Iniciales"/>
+    <tableColumn dataDxfId="22" id="4" name="Entradas"/>
+    <tableColumn dataDxfId="21" id="5" name="Salidas"/>
+    <tableColumn dataDxfId="20" id="6" name="Stock" totalsRowFunction="sum"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Entradas" displayName="Entradas" ref="A1:G3" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="18" displayName="Entradas" headerRowCount="1" headerRowDxfId="19" id="2" name="Entradas" ref="A1:G3">
   <autoFilter ref="A1:G3"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Num de Factura" totalsRowLabel="Total" dataDxfId="17"/>
-    <tableColumn id="2" name="Fecha" dataDxfId="16"/>
-    <tableColumn id="3" name="Codigo de Producto" dataDxfId="15"/>
-    <tableColumn id="4" name="Descripcion" dataDxfId="14"/>
-    <tableColumn id="5" name="Cantidad" totalsRowFunction="count" dataDxfId="13"/>
-    <tableColumn id="6" name="SERIE" dataDxfId="12"/>
-    <tableColumn id="7" name="OBSERVACIONES" dataDxfId="11"/>
+    <tableColumn dataDxfId="17" id="1" name="Num de Factura" totalsRowLabel="Total"/>
+    <tableColumn dataDxfId="16" id="2" name="Fecha"/>
+    <tableColumn dataDxfId="15" id="3" name="Codigo de Producto"/>
+    <tableColumn dataDxfId="14" id="4" name="Descripcion"/>
+    <tableColumn dataDxfId="13" id="5" name="Cantidad" totalsRowFunction="count"/>
+    <tableColumn dataDxfId="12" id="6" name="SERIE"/>
+    <tableColumn dataDxfId="11" id="7" name="OBSERVACIONES"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight12" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Salidas" displayName="Salidas" ref="A1:I3" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Salidas" headerRowCount="1" headerRowDxfId="9" id="3" name="Salidas" ref="A1:I3" totalsRowShown="0">
   <autoFilter ref="A1:I3"/>
   <sortState ref="A2:I3">
     <sortCondition ref="B1:B3"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Num de Factura" dataDxfId="8"/>
-    <tableColumn id="2" name="Fecha" dataDxfId="7"/>
-    <tableColumn id="3" name="Codigo Producto" dataDxfId="6"/>
-    <tableColumn id="4" name="Descripcion(Producto)" dataDxfId="5"/>
-    <tableColumn id="5" name="Cantidad" dataDxfId="4"/>
-    <tableColumn id="6" name="OBSERVACIONES" dataDxfId="3"/>
-    <tableColumn id="7" name="DE O P/CLIENTE" dataDxfId="2"/>
-    <tableColumn id="8" name="TECNICO RECIBIO Y FIRMO SALIDA" dataDxfId="1"/>
-    <tableColumn id="9" name="Serie" dataDxfId="0"/>
+    <tableColumn dataDxfId="8" id="1" name="Num de Factura"/>
+    <tableColumn dataDxfId="7" id="2" name="Fecha"/>
+    <tableColumn dataDxfId="6" id="3" name="Codigo Producto"/>
+    <tableColumn dataDxfId="5" id="4" name="Descripcion(Producto)"/>
+    <tableColumn dataDxfId="4" id="5" name="Cantidad"/>
+    <tableColumn dataDxfId="3" id="6" name="OBSERVACIONES"/>
+    <tableColumn dataDxfId="2" id="7" name="DE O P/CLIENTE"/>
+    <tableColumn dataDxfId="1" id="8" name="TECNICO RECIBIO Y FIRMO SALIDA"/>
+    <tableColumn dataDxfId="0" id="9" name="Serie"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -557,27 +562,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="8" customWidth="1"/>
-    <col min="7" max="8" width="12" style="7" customWidth="1"/>
-    <col min="9" max="58" width="11.42578125" style="7" customWidth="1"/>
-    <col min="59" max="16384" width="11.42578125" style="7"/>
+    <col customWidth="1" max="1" min="1" style="6" width="20.140625"/>
+    <col customWidth="1" max="2" min="2" style="8" width="39.85546875"/>
+    <col customWidth="1" max="3" min="3" style="8" width="20.140625"/>
+    <col customWidth="1" max="4" min="4" style="8" width="12"/>
+    <col customWidth="1" max="5" min="5" style="8" width="14.42578125"/>
+    <col customWidth="1" max="6" min="6" style="8" width="16.140625"/>
+    <col customWidth="1" max="8" min="7" style="7" width="12"/>
+    <col customWidth="1" max="58" min="9" style="7" width="11.42578125"/>
+    <col customWidth="1" max="16384" min="59" style="7" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.75" r="1" s="6" spans="1:6">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -597,40 +606,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>90</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8000</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -639,72 +676,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="5" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="5" width="14.5703125"/>
+    <col customWidth="1" max="2" min="2" style="5" width="17.85546875"/>
+    <col customWidth="1" max="3" min="3" style="5" width="22.5703125"/>
+    <col customWidth="1" max="4" min="4" style="5" width="17.28515625"/>
+    <col customWidth="1" max="5" min="5" style="5" width="15.28515625"/>
+    <col customWidth="1" max="7" min="7" style="5" width="15.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="33.75" r="1" s="3" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="9" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Solo Numeros" error="Esta celda solo acepta numeros" sqref="A1:A4 A7:A9 A11:A1048576"/>
+    <dataValidation allowBlank="0" error="Esta celda solo acepta numeros" errorTitle="Solo Numeros" showErrorMessage="1" showInputMessage="1" sqref="A1:A4 A7:A9 A11:A1048576"/>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -712,151 +753,68 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" style="5" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="4" width="17.5703125"/>
+    <col customWidth="1" max="2" min="2" style="4" width="14.28515625"/>
+    <col customWidth="1" max="3" min="3" style="4" width="21.28515625"/>
+    <col customWidth="1" max="4" min="4" style="4" width="21.140625"/>
+    <col customWidth="1" max="5" min="5" style="4" width="15.140625"/>
+    <col customWidth="1" max="6" min="6" style="5" width="27.7109375"/>
+    <col customWidth="1" max="7" min="7" style="5" width="26.85546875"/>
+    <col customWidth="1" max="8" min="8" style="5" width="31.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="33" r="1" s="3" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3" s="10"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="10" t="n"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:D1048576 D1 D3">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule dxfId="10" operator="equal" priority="1" type="cellIs">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
LA ELIMINACION DE DATOS ESTA SOLUCIONADO AHORA SOLO FALTA CARGAR A EXCEL
</commit_message>
<xml_diff>
--- a/polls/static/polls/Datos/Inventario.xlsx
+++ b/polls/static/polls/Datos/Inventario.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Israel\Desktop\tutorial\mysite\polls\static\polls\Datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7680" windowWidth="10170" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="inventario" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Entradas" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Salidas" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="inventario" sheetId="1" r:id="rId1"/>
+    <sheet name="Entradas" sheetId="2" r:id="rId2"/>
+    <sheet name="Salidas" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Inventario">Tabla31[]</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>CLASIF.EQUIP(ID)</t>
   </si>
@@ -92,20 +98,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -121,39 +126,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
@@ -187,7 +192,7 @@
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <numFmt formatCode=";;;" numFmtId="164"/>
+      <numFmt numFmtId="164" formatCode=";;;"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
@@ -244,59 +249,67 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="27" displayName="Tabla31" headerRowCount="1" headerRowDxfId="28" id="1" name="Tabla31" ref="A1:F3" totalsRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla31" displayName="Tabla31" ref="A1:F3" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
   <autoFilter ref="A1:F3"/>
   <tableColumns count="6">
-    <tableColumn dataDxfId="25" id="1" name="CLASIF.EQUIP(ID)" totalsRowLabel="Total"/>
-    <tableColumn dataDxfId="24" id="2" name="Descripcion"/>
-    <tableColumn dataDxfId="23" id="3" name="Existencias Iniciales"/>
-    <tableColumn dataDxfId="22" id="4" name="Entradas"/>
-    <tableColumn dataDxfId="21" id="5" name="Salidas"/>
-    <tableColumn dataDxfId="20" id="6" name="Stock" totalsRowFunction="sum"/>
+    <tableColumn id="1" name="CLASIF.EQUIP(ID)" totalsRowLabel="Total" dataDxfId="25"/>
+    <tableColumn id="2" name="Descripcion" dataDxfId="24"/>
+    <tableColumn id="3" name="Existencias Iniciales" dataDxfId="23"/>
+    <tableColumn id="4" name="Entradas" dataDxfId="22"/>
+    <tableColumn id="5" name="Salidas" dataDxfId="21"/>
+    <tableColumn id="6" name="Stock" totalsRowFunction="sum" dataDxfId="20"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="18" displayName="Entradas" headerRowCount="1" headerRowDxfId="19" id="2" name="Entradas" ref="A1:G3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Entradas" displayName="Entradas" ref="A1:G3" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:G3"/>
   <tableColumns count="7">
-    <tableColumn dataDxfId="17" id="1" name="Num de Factura" totalsRowLabel="Total"/>
-    <tableColumn dataDxfId="16" id="2" name="Fecha"/>
-    <tableColumn dataDxfId="15" id="3" name="Codigo de Producto"/>
-    <tableColumn dataDxfId="14" id="4" name="Descripcion"/>
-    <tableColumn dataDxfId="13" id="5" name="Cantidad" totalsRowFunction="count"/>
-    <tableColumn dataDxfId="12" id="6" name="SERIE"/>
-    <tableColumn dataDxfId="11" id="7" name="OBSERVACIONES"/>
+    <tableColumn id="1" name="Num de Factura" totalsRowLabel="Total" dataDxfId="17"/>
+    <tableColumn id="2" name="Fecha" dataDxfId="16"/>
+    <tableColumn id="3" name="Codigo de Producto" dataDxfId="15"/>
+    <tableColumn id="4" name="Descripcion" dataDxfId="14"/>
+    <tableColumn id="5" name="Cantidad" totalsRowFunction="count" dataDxfId="13"/>
+    <tableColumn id="6" name="SERIE" dataDxfId="12"/>
+    <tableColumn id="7" name="OBSERVACIONES" dataDxfId="11"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Salidas" headerRowCount="1" headerRowDxfId="9" id="3" name="Salidas" ref="A1:I3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Salidas" displayName="Salidas" ref="A1:I3" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:I3"/>
   <sortState ref="A2:I3">
     <sortCondition ref="B1:B3"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn dataDxfId="8" id="1" name="Num de Factura"/>
-    <tableColumn dataDxfId="7" id="2" name="Fecha"/>
-    <tableColumn dataDxfId="6" id="3" name="Codigo Producto"/>
-    <tableColumn dataDxfId="5" id="4" name="Descripcion(Producto)"/>
-    <tableColumn dataDxfId="4" id="5" name="Cantidad"/>
-    <tableColumn dataDxfId="3" id="6" name="OBSERVACIONES"/>
-    <tableColumn dataDxfId="2" id="7" name="DE O P/CLIENTE"/>
-    <tableColumn dataDxfId="1" id="8" name="TECNICO RECIBIO Y FIRMO SALIDA"/>
-    <tableColumn dataDxfId="0" id="9" name="Serie"/>
+    <tableColumn id="1" name="Num de Factura" dataDxfId="8"/>
+    <tableColumn id="2" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="3" name="Codigo Producto" dataDxfId="6"/>
+    <tableColumn id="4" name="Descripcion(Producto)" dataDxfId="5"/>
+    <tableColumn id="5" name="Cantidad" dataDxfId="4"/>
+    <tableColumn id="6" name="OBSERVACIONES" dataDxfId="3"/>
+    <tableColumn id="7" name="DE O P/CLIENTE" dataDxfId="2"/>
+    <tableColumn id="8" name="TECNICO RECIBIO Y FIRMO SALIDA" dataDxfId="1"/>
+    <tableColumn id="9" name="Serie" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -562,31 +575,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="6" width="20.140625"/>
-    <col customWidth="1" max="2" min="2" style="8" width="39.85546875"/>
-    <col customWidth="1" max="3" min="3" style="8" width="20.140625"/>
-    <col customWidth="1" max="4" min="4" style="8" width="12"/>
-    <col customWidth="1" max="5" min="5" style="8" width="14.42578125"/>
-    <col customWidth="1" max="6" min="6" style="8" width="16.140625"/>
-    <col customWidth="1" max="8" min="7" style="7" width="12"/>
-    <col customWidth="1" max="58" min="9" style="7" width="11.42578125"/>
-    <col customWidth="1" max="16384" min="59" style="7" width="11.42578125"/>
+    <col min="1" max="1" width="20.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" customWidth="1"/>
+    <col min="7" max="8" width="12" style="7" customWidth="1"/>
+    <col min="9" max="59" width="11.42578125" style="7" customWidth="1"/>
+    <col min="60" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.75" r="1" s="6" spans="1:6">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -606,68 +615,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="7">
         <v>50</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="7">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>90</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>8000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>8000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -676,28 +685,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="5" width="14.5703125"/>
-    <col customWidth="1" max="2" min="2" style="5" width="17.85546875"/>
-    <col customWidth="1" max="3" min="3" style="5" width="22.5703125"/>
-    <col customWidth="1" max="4" min="4" style="5" width="17.28515625"/>
-    <col customWidth="1" max="5" min="5" style="5" width="15.28515625"/>
-    <col customWidth="1" max="7" min="7" style="5" width="15.7109375"/>
+    <col min="1" max="1" width="14.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="33.75" r="1" s="3" spans="1:7">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -720,32 +725,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="3" t="n"/>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="n"/>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="9" t="n"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="0" error="Esta celda solo acepta numeros" errorTitle="Solo Numeros" showErrorMessage="1" showInputMessage="1" sqref="A1:A4 A7:A9 A11:A1048576"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Solo Numeros" error="Esta celda solo acepta numeros" sqref="A1:A4 A7:A9 A11:A1048576"/>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -753,30 +758,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="17.5703125"/>
-    <col customWidth="1" max="2" min="2" style="4" width="14.28515625"/>
-    <col customWidth="1" max="3" min="3" style="4" width="21.28515625"/>
-    <col customWidth="1" max="4" min="4" style="4" width="21.140625"/>
-    <col customWidth="1" max="5" min="5" style="4" width="15.140625"/>
-    <col customWidth="1" max="6" min="6" style="5" width="27.7109375"/>
-    <col customWidth="1" max="7" min="7" style="5" width="26.85546875"/>
-    <col customWidth="1" max="8" min="8" style="5" width="31.5703125"/>
+    <col min="1" max="1" width="17.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="33" r="1" s="3" spans="1:9">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -805,16 +806,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="B3" s="10" t="n"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:D1048576 D1 D3">
-    <cfRule dxfId="10" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Terminado Esperando que hagan prueba de escritorio
</commit_message>
<xml_diff>
--- a/polls/static/polls/Datos/Inventario.xlsx
+++ b/polls/static/polls/Datos/Inventario.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Israel\Desktop\tutorial\mysite\polls\static\polls\Datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7680" windowWidth="10170" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="7680"/>
   </bookViews>
   <sheets>
-    <sheet name="inventario" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Entradas" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Salidas" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="inventario" sheetId="1" r:id="rId1"/>
+    <sheet name="Entradas" sheetId="2" r:id="rId2"/>
+    <sheet name="Salidas" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Inventario">Tabla31[]</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>CLASIF.EQUIP(ID)</t>
   </si>
@@ -36,24 +42,6 @@
   </si>
   <si>
     <t>Stock</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Carr</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>Trailer</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>Ford Focus</t>
   </si>
   <si>
     <t>Num de Factura</t>
@@ -92,20 +80,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -121,39 +108,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
@@ -187,7 +174,7 @@
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <numFmt formatCode=";;;" numFmtId="164"/>
+      <numFmt numFmtId="164" formatCode=";;;"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
@@ -244,59 +231,67 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="27" displayName="Tabla31" headerRowCount="1" headerRowDxfId="28" id="1" name="Tabla31" ref="A1:F3" totalsRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla31" displayName="Tabla31" ref="A1:F3" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
   <autoFilter ref="A1:F3"/>
   <tableColumns count="6">
-    <tableColumn dataDxfId="25" id="1" name="CLASIF.EQUIP(ID)" totalsRowLabel="Total"/>
-    <tableColumn dataDxfId="24" id="2" name="Descripcion"/>
-    <tableColumn dataDxfId="23" id="3" name="Existencias Iniciales"/>
-    <tableColumn dataDxfId="22" id="4" name="Entradas"/>
-    <tableColumn dataDxfId="21" id="5" name="Salidas"/>
-    <tableColumn dataDxfId="20" id="6" name="Stock" totalsRowFunction="sum"/>
+    <tableColumn id="1" name="CLASIF.EQUIP(ID)" totalsRowLabel="Total" dataDxfId="25"/>
+    <tableColumn id="2" name="Descripcion" dataDxfId="24"/>
+    <tableColumn id="3" name="Existencias Iniciales" dataDxfId="23"/>
+    <tableColumn id="4" name="Entradas" dataDxfId="22"/>
+    <tableColumn id="5" name="Salidas" dataDxfId="21"/>
+    <tableColumn id="6" name="Stock" totalsRowFunction="sum" dataDxfId="20"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="18" displayName="Entradas" headerRowCount="1" headerRowDxfId="19" id="2" name="Entradas" ref="A1:G3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Entradas" displayName="Entradas" ref="A1:G3" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:G3"/>
   <tableColumns count="7">
-    <tableColumn dataDxfId="17" id="1" name="Num de Factura" totalsRowLabel="Total"/>
-    <tableColumn dataDxfId="16" id="2" name="Fecha"/>
-    <tableColumn dataDxfId="15" id="3" name="Codigo de Producto"/>
-    <tableColumn dataDxfId="14" id="4" name="Descripcion"/>
-    <tableColumn dataDxfId="13" id="5" name="Cantidad" totalsRowFunction="count"/>
-    <tableColumn dataDxfId="12" id="6" name="SERIE"/>
-    <tableColumn dataDxfId="11" id="7" name="OBSERVACIONES"/>
+    <tableColumn id="1" name="Num de Factura" totalsRowLabel="Total" dataDxfId="17"/>
+    <tableColumn id="2" name="Fecha" dataDxfId="16"/>
+    <tableColumn id="3" name="Codigo de Producto" dataDxfId="15"/>
+    <tableColumn id="4" name="Descripcion" dataDxfId="14"/>
+    <tableColumn id="5" name="Cantidad" totalsRowFunction="count" dataDxfId="13"/>
+    <tableColumn id="6" name="SERIE" dataDxfId="12"/>
+    <tableColumn id="7" name="OBSERVACIONES" dataDxfId="11"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Salidas" headerRowCount="1" headerRowDxfId="9" id="3" name="Salidas" ref="A1:I3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Salidas" displayName="Salidas" ref="A1:I3" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:I3"/>
   <sortState ref="A2:I3">
     <sortCondition ref="B1:B3"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn dataDxfId="8" id="1" name="Num de Factura"/>
-    <tableColumn dataDxfId="7" id="2" name="Fecha"/>
-    <tableColumn dataDxfId="6" id="3" name="Codigo Producto"/>
-    <tableColumn dataDxfId="5" id="4" name="Descripcion(Producto)"/>
-    <tableColumn dataDxfId="4" id="5" name="Cantidad"/>
-    <tableColumn dataDxfId="3" id="6" name="OBSERVACIONES"/>
-    <tableColumn dataDxfId="2" id="7" name="DE O P/CLIENTE"/>
-    <tableColumn dataDxfId="1" id="8" name="TECNICO RECIBIO Y FIRMO SALIDA"/>
-    <tableColumn dataDxfId="0" id="9" name="Serie"/>
+    <tableColumn id="1" name="Num de Factura" dataDxfId="8"/>
+    <tableColumn id="2" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="3" name="Codigo Producto" dataDxfId="6"/>
+    <tableColumn id="4" name="Descripcion(Producto)" dataDxfId="5"/>
+    <tableColumn id="5" name="Cantidad" dataDxfId="4"/>
+    <tableColumn id="6" name="OBSERVACIONES" dataDxfId="3"/>
+    <tableColumn id="7" name="DE O P/CLIENTE" dataDxfId="2"/>
+    <tableColumn id="8" name="TECNICO RECIBIO Y FIRMO SALIDA" dataDxfId="1"/>
+    <tableColumn id="9" name="Serie" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -562,31 +557,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="6" width="20.140625"/>
-    <col customWidth="1" max="2" min="2" style="8" width="39.85546875"/>
-    <col customWidth="1" max="3" min="3" style="8" width="20.140625"/>
-    <col customWidth="1" max="4" min="4" style="8" width="12"/>
-    <col customWidth="1" max="5" min="5" style="8" width="14.42578125"/>
-    <col customWidth="1" max="6" min="6" style="8" width="16.140625"/>
-    <col customWidth="1" max="8" min="7" style="7" width="12"/>
-    <col customWidth="1" max="60" min="9" style="7" width="11.42578125"/>
-    <col customWidth="1" max="16384" min="61" style="7" width="11.42578125"/>
+    <col min="1" max="1" width="20.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" customWidth="1"/>
+    <col min="7" max="8" width="12" style="7" customWidth="1"/>
+    <col min="9" max="63" width="11.42578125" style="7" customWidth="1"/>
+    <col min="64" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.75" r="1" s="6" spans="1:6">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -606,68 +597,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>90</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>8005</v>
-      </c>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -676,76 +623,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="5" width="14.5703125"/>
-    <col customWidth="1" max="2" min="2" style="5" width="17.85546875"/>
-    <col customWidth="1" max="3" min="3" style="5" width="22.5703125"/>
-    <col customWidth="1" max="4" min="4" style="5" width="17.28515625"/>
-    <col customWidth="1" max="5" min="5" style="5" width="15.28515625"/>
-    <col customWidth="1" max="7" min="7" style="5" width="15.7109375"/>
+    <col min="1" max="1" width="14.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="33.75" r="1" s="3" spans="1:7">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="3" t="n"/>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="n"/>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="9" t="n"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8" s="9"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="G20"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="0" error="Esta celda solo acepta numeros" errorTitle="Solo Numeros" showErrorMessage="1" showInputMessage="1" sqref="A1:A4 A7:A9 A11:A1048576"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Solo Numeros" error="Esta celda solo acepta numeros" sqref="A1:A4 A7:A9 A11:A1048576"/>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -753,68 +829,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="17.5703125"/>
-    <col customWidth="1" max="2" min="2" style="4" width="14.28515625"/>
-    <col customWidth="1" max="3" min="3" style="4" width="21.28515625"/>
-    <col customWidth="1" max="4" min="4" style="4" width="21.140625"/>
-    <col customWidth="1" max="5" min="5" style="4" width="15.140625"/>
-    <col customWidth="1" max="6" min="6" style="5" width="27.7109375"/>
-    <col customWidth="1" max="7" min="7" style="5" width="26.85546875"/>
-    <col customWidth="1" max="8" min="8" style="5" width="31.5703125"/>
+    <col min="1" max="1" width="17.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="33" r="1" s="3" spans="1:9">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="B3" s="10" t="n"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:D1048576 D1 D3">
-    <cfRule dxfId="10" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>